<commit_message>
excel and ppt export primary version
</commit_message>
<xml_diff>
--- a/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/SingleTableForPPT.xlsx
+++ b/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/SingleTableForPPT.xlsx
@@ -61,7 +61,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +77,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB6DEE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -108,24 +114,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,8 +165,8 @@
       <xdr:rowOff>22243</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6331</xdr:rowOff>
     </xdr:to>
@@ -482,384 +491,607 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:S29"/>
+  <dimension ref="A3:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="3" customWidth="1"/>
-    <col min="2" max="19" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="4" max="15" width="10.140625" customWidth="1"/>
+    <col min="16" max="19" width="10.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="1"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="13"/>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-    </row>
-    <row r="7" spans="1:19" s="9" customFormat="1" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:19" s="3" customFormat="1" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
     </row>
     <row r="8" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
     </row>
     <row r="9" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
     </row>
     <row r="10" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
     </row>
     <row r="11" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
     </row>
     <row r="12" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
     </row>
     <row r="13" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
     </row>
     <row r="14" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
     </row>
     <row r="15" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
     </row>
     <row r="16" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
     </row>
     <row r="17" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
     </row>
     <row r="18" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
     </row>
     <row r="20" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
     </row>
     <row r="21" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
     </row>
     <row r="22" spans="1:19" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
     </row>
-    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+    </row>
+    <row r="29" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>